<commit_message>
app trader final commit
</commit_message>
<xml_diff>
--- a/data/app_store games visual.xlsx
+++ b/data/app_store games visual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RMAUR\Documents\nss-data-analytics\Projects\app-trader-the-v-lookup-velociraptors\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35FF779-8299-45C5-A2E1-8E6A9785DE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F11D3F-09E6-4B2D-8845-637F4C304D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{2DCB4CB0-4C60-4A97-BBCD-8A2DD54C1A36}"/>
   </bookViews>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -511,7 +511,7 @@
         <v>100072472</v>
       </c>
       <c r="C2">
-        <v>20000</v>
+        <v>1051105.8799999999</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -522,7 +522,7 @@
         <v>87989863</v>
       </c>
       <c r="C3">
-        <v>21466.67</v>
+        <v>1043333.33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -533,7 +533,7 @@
         <v>79219668</v>
       </c>
       <c r="C4">
-        <v>43581.82</v>
+        <v>1012854.55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -544,7 +544,7 @@
         <v>52603666</v>
       </c>
       <c r="C5">
-        <v>32623.33</v>
+        <v>1018576.67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -555,7 +555,7 @@
         <v>34835983</v>
       </c>
       <c r="C6">
-        <v>24141.67</v>
+        <v>1034258.33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -566,7 +566,7 @@
         <v>12798545</v>
       </c>
       <c r="C7">
-        <v>39955.56</v>
+        <v>1044844.44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -577,7 +577,7 @@
         <v>11445045</v>
       </c>
       <c r="C8">
-        <v>54200</v>
+        <v>902371.43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -588,7 +588,7 @@
         <v>10308841</v>
       </c>
       <c r="C9">
-        <v>22200</v>
+        <v>1029000</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -599,7 +599,7 @@
         <v>9962579</v>
       </c>
       <c r="C10">
-        <v>31063.64</v>
+        <v>1031263.64</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -610,7 +610,7 @@
         <v>9835155</v>
       </c>
       <c r="C11">
-        <v>69000</v>
+        <v>995290.91</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -621,7 +621,7 @@
         <v>6821242</v>
       </c>
       <c r="C12">
-        <v>20000</v>
+        <v>1060000</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -632,7 +632,7 @@
         <v>4637302</v>
       </c>
       <c r="C13">
-        <v>59900</v>
+        <v>976900</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -643,7 +643,7 @@
         <v>2442236</v>
       </c>
       <c r="C14">
-        <v>20000</v>
+        <v>995200</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -654,7 +654,7 @@
         <v>1650667</v>
       </c>
       <c r="C15">
-        <v>20000</v>
+        <v>1038400</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -665,7 +665,7 @@
         <v>1346250</v>
       </c>
       <c r="C16">
-        <v>24950</v>
+        <v>1033450</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -676,7 +676,7 @@
         <v>1168801</v>
       </c>
       <c r="C17">
-        <v>39900</v>
+        <v>1040100</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -687,7 +687,7 @@
         <v>1042617</v>
       </c>
       <c r="C18">
-        <v>20000</v>
+        <v>1060000</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -698,7 +698,7 @@
         <v>965675</v>
       </c>
       <c r="C19">
-        <v>29900</v>
+        <v>1060900</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -709,7 +709,7 @@
         <v>725315</v>
       </c>
       <c r="C20">
-        <v>20000</v>
+        <v>1027600</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -720,7 +720,7 @@
         <v>679740</v>
       </c>
       <c r="C21">
-        <v>20000</v>
+        <v>1060000</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -731,7 +731,7 @@
         <v>678241</v>
       </c>
       <c r="C22">
-        <v>20000</v>
+        <v>973600</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -742,7 +742,7 @@
         <v>534519</v>
       </c>
       <c r="C23">
-        <v>20000</v>
+        <v>1016800</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -753,7 +753,7 @@
         <v>425128</v>
       </c>
       <c r="C24">
-        <v>20000</v>
+        <v>962800</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -764,7 +764,7 @@
         <v>390214</v>
       </c>
       <c r="C25">
-        <v>59900</v>
+        <v>998500</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -775,7 +775,7 @@
         <v>126015</v>
       </c>
       <c r="C26">
-        <v>20000</v>
+        <v>844000</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -786,7 +786,7 @@
         <v>78092</v>
       </c>
       <c r="C27">
-        <v>99800</v>
+        <v>915400</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -797,7 +797,7 @@
         <v>77038</v>
       </c>
       <c r="C28">
-        <v>20000</v>
+        <v>1060000</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -808,7 +808,7 @@
         <v>73776</v>
       </c>
       <c r="C29">
-        <v>20000</v>
+        <v>952000</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
@@ -819,7 +819,7 @@
         <v>35449</v>
       </c>
       <c r="C30">
-        <v>79800</v>
+        <v>978600</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
@@ -830,7 +830,7 @@
         <v>2734</v>
       </c>
       <c r="C31">
-        <v>59800</v>
+        <v>1041800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>